<commit_message>
Ajusto con el ppt y specs
</commit_message>
<xml_diff>
--- a/Ejemplo de Entregas Gratuitas.xlsx
+++ b/Ejemplo de Entregas Gratuitas.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
-  <si>
-    <t xml:space="preserve">        Se ofrece entregas gratuitas a clientes premium una vez que compran cierta cantidad de libros.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        La entrega gratuita no se ofrece a clientes normales o clientes premium que compran otro tipo de producto.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>categoria</t>
   </si>
@@ -54,9 +48,6 @@
     <t>digital</t>
   </si>
   <si>
-    <t>precio</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -179,13 +170,47 @@
       </rPr>
       <t>categoria</t>
     </r>
+  </si>
+  <si>
+    <t>Se ofrece entregas gratuitas a clientes premium basado en un precio mínimo.</t>
+  </si>
+  <si>
+    <t>La entrega gratuita no se ofrece a clientes normales o a clientes premium cuyas órdenes contienen bienes digitales.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>que el mínimo para entrega gratuita es de $25</t>
+  </si>
+  <si>
+    <t>precio total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intención del ejemplo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">clientes normales nunca aplican   </t>
+  </si>
+  <si>
+    <t>clientes premium tienen promocion de envío en libros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">las lavadoras no se entregan gratis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bienes digitales no aplican     </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +253,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,21 +278,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -274,13 +317,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A12:E16" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A12:E16"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B13:G17" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="B13:G17"/>
+  <tableColumns count="6">
+    <tableColumn id="6" name="intención del ejemplo " dataCellStyle="Normal"/>
     <tableColumn id="1" name="categoria" dataCellStyle="Normal"/>
     <tableColumn id="2" name="cantidad" dataCellStyle="Normal"/>
     <tableColumn id="3" name=" productos" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="precio" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="precio total" dataDxfId="0" dataCellStyle="Currency"/>
     <tableColumn id="5" name="podria tener una entrega gratuita" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -542,7 +586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,167 +594,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4">
+        <v>250</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="4">
+        <v>250</v>
+      </c>
+      <c r="G17" t="s">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>250</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>250</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agrego Excel del ejemplo de Entregas Gratuitas
</commit_message>
<xml_diff>
--- a/Ejemplo de Entregas Gratuitas.xlsx
+++ b/Ejemplo de Entregas Gratuitas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejemplos base" sheetId="2" r:id="rId1"/>
+    <sheet name="Refinado" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>categoria</t>
   </si>
@@ -87,6 +88,33 @@
     <t>Entonces</t>
   </si>
   <si>
+    <t>Se ofrece entregas gratuitas a clientes premium basado en un precio mínimo.</t>
+  </si>
+  <si>
+    <t>La entrega gratuita no se ofrece a clientes normales o a clientes premium cuyas órdenes contienen bienes digitales.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>precio total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intención del ejemplo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">clientes normales nunca aplican   </t>
+  </si>
+  <si>
+    <t>clientes premium tienen promocion de envío en libros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">las lavadoras no se entregan gratis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bienes digitales no aplican     </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -95,7 +123,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>la orden contiene una </t>
+      <t>la orden contiene una "</t>
     </r>
     <r>
       <rPr>
@@ -105,7 +133,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>cantidad</t>
+      <t>cantidad"</t>
     </r>
     <r>
       <rPr>
@@ -115,7 +143,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t> de </t>
+      <t> de "</t>
     </r>
     <r>
       <rPr>
@@ -125,7 +153,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>productos</t>
+      <t>productos"</t>
     </r>
     <r>
       <rPr>
@@ -145,8 +173,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>precio total</t>
-    </r>
+      <t>precio total"</t>
+    </r>
+  </si>
+  <si>
+    <t>"podria tener una entrega gratuita"</t>
   </si>
   <si>
     <r>
@@ -157,49 +188,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>un cliente de cierta </t>
+      <t>un cliente de cierta "</t>
     </r>
     <r>
       <rPr>
-        <i/>
         <sz val="11"/>
         <color rgb="FFA31515"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>categoria</t>
-    </r>
-  </si>
-  <si>
-    <t>Se ofrece entregas gratuitas a clientes premium basado en un precio mínimo.</t>
-  </si>
-  <si>
-    <t>La entrega gratuita no se ofrece a clientes normales o a clientes premium cuyas órdenes contienen bienes digitales.</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>que el mínimo para entrega gratuita es de $25</t>
-  </si>
-  <si>
-    <t>precio total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intención del ejemplo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">clientes normales nunca aplican   </t>
-  </si>
-  <si>
-    <t>clientes premium tienen promocion de envío en libros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">las lavadoras no se entregan gratis  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bienes digitales no aplican     </t>
+      <t>categoria"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>que el mínimo para entrega gratuita es de "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Ejemplos</t>
   </si>
 </sst>
 </file>
@@ -208,9 +236,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,14 +255,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFA31515"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,16 +280,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -277,23 +318,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -301,7 +395,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -317,8 +411,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B13:G17" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="B13:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B12:G16" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="B12:G16"/>
   <tableColumns count="6">
     <tableColumn id="6" name="intención del ejemplo " dataCellStyle="Normal"/>
     <tableColumn id="1" name="categoria" dataCellStyle="Normal"/>
@@ -586,7 +680,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,15 +688,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10">
+        <v>25</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="10">
+        <v>50</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="10">
+        <v>250</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12">
+        <v>250</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -621,77 +845,101 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
+      <c r="B8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -699,86 +947,66 @@
       <c r="E14" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4">
-        <v>50</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>28</v>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="4">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3">
         <v>250</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4">
-        <v>250</v>
-      </c>
-      <c r="G17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>